<commit_message>
working full input parsing
</commit_message>
<xml_diff>
--- a/src/assets/sample-input.xlsx
+++ b/src/assets/sample-input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-repos\board-game-helper\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\board-game-helper\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C0BCC7-0575-4E57-AD0D-D2CB2C936B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08C1B03-B519-4CD3-B170-10A04995BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5E032DFC-9EF6-48F7-A30E-73951A4845B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5E032DFC-9EF6-48F7-A30E-73951A4845B9}"/>
   </bookViews>
   <sheets>
     <sheet name="players" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -521,7 +521,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +736,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80F9D70-3A8A-4C43-A789-F330CE79F43B}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -744,13 +744,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -785,6 +785,32 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>